<commit_message>
Add `task-3` in `game-theory`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-1/task-1.xlsx
+++ b/3-course-6-semester/econometrics/task-1/task-1.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\econometrics\task-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69A0F05-F4B7-4ABF-B122-FAD5606B655F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659854B9-9368-4AAB-8785-0630DF92E40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{110B23AD-468D-4208-8880-E2E080976DA8}"/>
+    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{110B23AD-468D-4208-8880-E2E080976DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Занятие 1" sheetId="1" r:id="rId1"/>
     <sheet name="Домашнее задание 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -382,7 +383,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000%"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -837,9 +838,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,11 +873,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
@@ -910,18 +905,6 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -940,8 +923,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2479,8 +2480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5342DA5F-1EB0-415F-98F9-15D5C27AB455}">
   <dimension ref="A2:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,117 +2498,117 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>28</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>31</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>39</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>26</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>55</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>43</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>44</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>57</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>53</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>66</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>90</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
+      <c r="A16" s="17">
         <v>95</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="18">
         <v>105</v>
       </c>
     </row>
@@ -2637,14 +2638,14 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -3189,10 +3190,10 @@
       </c>
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E65" s="64" t="s">
+      <c r="E65" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="F65" s="64"/>
+      <c r="F65" s="60"/>
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F66">
@@ -3228,11 +3229,11 @@
       </c>
     </row>
     <row r="70" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E70" s="24">
+      <c r="E70" s="23">
         <f>F63-F69</f>
         <v>80.376097182463667</v>
       </c>
-      <c r="F70" s="24">
+      <c r="F70" s="23">
         <f>F63+F69</f>
         <v>116.0815373427989</v>
       </c>
@@ -3252,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63023E1B-49CB-46E7-86D3-D8D6E5AAD37A}">
   <dimension ref="B3:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3266,73 +3267,79 @@
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="22.7109375" customWidth="1"/>
     <col min="13" max="13" width="20.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
     <col min="15" max="15" width="15.42578125" customWidth="1"/>
     <col min="16" max="16" width="20.85546875" customWidth="1"/>
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="J3" s="25" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J3" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-    </row>
-    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="24" t="s">
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+    </row>
+    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
+    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>46</v>
       </c>
       <c r="J5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20">
+      <c r="P5">
+        <f>Q9/275</f>
+        <v>17.650909090909092</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19">
         <v>28</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>64</v>
       </c>
-      <c r="E6" s="28">
-        <f>LN(B6)</f>
+      <c r="E6" s="27">
+        <f t="shared" ref="E6:E17" si="0">LN(B6)</f>
         <v>3.3322045101752038</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <v>4.1588830833596715</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
         <v>31</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>62</v>
       </c>
-      <c r="E7" s="26">
-        <f>LN(B7)</f>
+      <c r="E7" s="25">
+        <f t="shared" si="0"/>
         <v>3.4339872044851463</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>4.1271343850450917</v>
       </c>
       <c r="J7" s="7" t="s">
@@ -3340,18 +3347,18 @@
       </c>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
         <v>39</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>65</v>
       </c>
-      <c r="E8" s="26">
-        <f>LN(B8)</f>
+      <c r="E8" s="25">
+        <f t="shared" si="0"/>
         <v>3.6635616461296463</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>4.1743872698956368</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -3361,18 +3368,18 @@
         <v>0.88750686904671994</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
         <v>26</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>68</v>
       </c>
-      <c r="E9" s="26">
-        <f>LN(B9)</f>
+      <c r="E9" s="25">
+        <f t="shared" si="0"/>
         <v>3.2580965380214821</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>4.219507705176107</v>
       </c>
       <c r="J9" s="4" t="s">
@@ -3381,19 +3388,23 @@
       <c r="K9" s="4">
         <v>0.78766844260511171</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="Q9">
+        <f>4854</f>
+        <v>4854</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
         <v>55</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>72</v>
       </c>
-      <c r="E10" s="26">
-        <f>LN(B10)</f>
+      <c r="E10" s="25">
+        <f t="shared" si="0"/>
         <v>4.0073331852324712</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="26">
         <v>4.2766661190160553</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -3402,19 +3413,26 @@
       <c r="K10" s="4">
         <v>0.7664352868656229</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <f>275*28</f>
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
         <v>43</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>82</v>
       </c>
-      <c r="E11" s="26">
-        <f>LN(B11)</f>
+      <c r="E11" s="25">
+        <f t="shared" si="0"/>
         <v>3.7612001156935624</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="26">
         <v>4.4067192472642533</v>
       </c>
       <c r="J11" s="4" t="s">
@@ -3423,19 +3441,22 @@
       <c r="K11" s="4">
         <v>9.0558540559564443E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16">
+      <c r="O11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15">
         <v>44</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>86</v>
       </c>
-      <c r="E12" s="26">
-        <f>LN(B12)</f>
+      <c r="E12" s="25">
+        <f t="shared" si="0"/>
         <v>3.784189633918261</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <v>4.4543472962535073</v>
       </c>
       <c r="J12" s="5" t="s">
@@ -3444,52 +3465,55 @@
       <c r="K12" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="O12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="15">
         <v>57</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>87</v>
       </c>
-      <c r="E13" s="26">
-        <f>LN(B13)</f>
+      <c r="E13" s="25">
+        <f t="shared" si="0"/>
         <v>4.0430512678345503</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <v>4.4659081186545837</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="16">
+    <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15">
         <v>53</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>91</v>
       </c>
-      <c r="E14" s="26">
-        <f>LN(B14)</f>
+      <c r="E14" s="25">
+        <f t="shared" si="0"/>
         <v>3.970291913552122</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="26">
         <v>4.5108595065168497</v>
       </c>
       <c r="J14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="15">
         <v>66</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>96</v>
       </c>
-      <c r="E15" s="26">
-        <f>LN(B15)</f>
+      <c r="E15" s="25">
+        <f t="shared" si="0"/>
         <v>4.1896547420264252</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>4.5643481914678361</v>
       </c>
       <c r="J15" s="6"/>
@@ -3509,18 +3533,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
         <v>90</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>101</v>
       </c>
-      <c r="E16" s="26">
-        <f>LN(B16)</f>
+      <c r="E16" s="25">
+        <f t="shared" si="0"/>
         <v>4.499809670330265</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="26">
         <v>4.6151205168412597</v>
       </c>
       <c r="J16" s="4" t="s">
@@ -3543,17 +3567,17 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <v>95</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="18">
         <v>105</v>
       </c>
-      <c r="E17" s="30">
-        <f>LN(B17)</f>
+      <c r="E17" s="29">
+        <f t="shared" si="0"/>
         <v>4.5538768916005408</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="30">
         <v>4.6539603501575231</v>
       </c>
       <c r="J17" s="4" t="s">
@@ -3614,10 +3638,10 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="34">
         <f>EXP(K21)</f>
         <v>17.314184802848953</v>
       </c>
@@ -3650,10 +3674,10 @@
       </c>
     </row>
     <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="63" t="s">
+      <c r="G22" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="37">
+      <c r="H22" s="35">
         <f>K22</f>
         <v>0.39592719431196294</v>
       </c>
@@ -3687,28 +3711,28 @@
     </row>
     <row r="23" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="36">
+      <c r="F24" s="34">
         <f>AVERAGE(E6:E17)</f>
         <v>3.8747714432499727</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="36">
         <f>AVERAGE(F6:F17)</f>
         <v>4.3856534824706985</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="38" cm="1">
+      <c r="F26" s="36" cm="1">
         <f t="array" ref="F26">AVERAGE(E6:E17*F6:F17)</f>
         <v>17.057436001798319</v>
       </c>
@@ -3717,24 +3741,24 @@
       </c>
     </row>
     <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="36">
         <f>VARPA(E6:E17)</f>
         <v>0.1617245009965384</v>
       </c>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
     </row>
     <row r="28" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="63" t="s">
+      <c r="E28" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="35">
         <f>VARPA(F6:F17)</f>
         <v>3.2185705887273292E-2</v>
       </c>
@@ -3747,24 +3771,24 @@
       <c r="L28" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M28" s="47" t="s">
+      <c r="M28" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="N28" s="47" t="s">
+      <c r="N28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="O28" s="47" t="s">
+      <c r="O28" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="P28" s="47" t="s">
+      <c r="P28" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="Q28" s="47" t="s">
+      <c r="Q28" s="45" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F29" s="33"/>
+      <c r="F29" s="32"/>
       <c r="J29" s="4">
         <v>1</v>
       </c>
@@ -3774,28 +3798,28 @@
       <c r="L29" s="4">
         <v>-1.1953395572287029E-2</v>
       </c>
-      <c r="M29" s="48">
+      <c r="M29" s="46">
         <f>EXP(K29)</f>
         <v>64.76960786658114</v>
       </c>
-      <c r="N29" s="48">
+      <c r="N29" s="46">
         <v>64</v>
       </c>
-      <c r="O29" s="48">
+      <c r="O29" s="46">
         <f>M29-N29</f>
         <v>0.76960786658113989</v>
       </c>
-      <c r="P29" s="48">
+      <c r="P29" s="46">
         <f>ABS(O29)</f>
         <v>0.76960786658113989</v>
       </c>
-      <c r="Q29" s="49">
+      <c r="Q29" s="47">
         <f>P29/N29</f>
         <v>1.2025122915330311E-2</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F30" s="33"/>
+      <c r="F30" s="32"/>
       <c r="J30" s="4">
         <v>2</v>
       </c>
@@ -3805,28 +3829,28 @@
       <c r="L30" s="4">
         <v>-8.4000630474514892E-2</v>
       </c>
-      <c r="M30" s="48">
-        <f t="shared" ref="M30:M40" si="0">EXP(K30)</f>
+      <c r="M30" s="46">
+        <f t="shared" ref="M30:M40" si="1">EXP(K30)</f>
         <v>67.433033930943182</v>
       </c>
-      <c r="N30" s="48">
+      <c r="N30" s="46">
         <v>62</v>
       </c>
-      <c r="O30" s="48">
-        <f t="shared" ref="O30:O40" si="1">M30-N30</f>
+      <c r="O30" s="46">
+        <f t="shared" ref="O30:O40" si="2">M30-N30</f>
         <v>5.4330339309431821</v>
       </c>
-      <c r="P30" s="48">
-        <f t="shared" ref="P30:P40" si="2">ABS(O30)</f>
+      <c r="P30" s="46">
+        <f t="shared" ref="P30:P40" si="3">ABS(O30)</f>
         <v>5.4330339309431821</v>
       </c>
-      <c r="Q30" s="49">
-        <f t="shared" ref="Q30:Q40" si="3">P30/N30</f>
+      <c r="Q30" s="47">
+        <f t="shared" ref="Q30:Q40" si="4">P30/N30</f>
         <v>8.762957953134165E-2</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F31" s="33"/>
+      <c r="F31" s="32"/>
       <c r="J31" s="4">
         <v>3</v>
       </c>
@@ -3836,28 +3860,28 @@
       <c r="L31" s="4">
         <v>-0.12764251019001183</v>
       </c>
-      <c r="M31" s="48">
-        <f t="shared" si="0"/>
+      <c r="M31" s="46">
+        <f t="shared" si="1"/>
         <v>73.84953999777764</v>
       </c>
-      <c r="N31" s="48">
+      <c r="N31" s="46">
         <v>65</v>
       </c>
-      <c r="O31" s="48">
-        <f t="shared" si="1"/>
-        <v>8.8495399977776401</v>
-      </c>
-      <c r="P31" s="48">
+      <c r="O31" s="46">
         <f t="shared" si="2"/>
         <v>8.8495399977776401</v>
       </c>
-      <c r="Q31" s="49">
+      <c r="P31" s="46">
         <f t="shared" si="3"/>
+        <v>8.8495399977776401</v>
+      </c>
+      <c r="Q31" s="47">
+        <f t="shared" si="4"/>
         <v>0.13614676919657909</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F32" s="33"/>
+      <c r="F32" s="32"/>
       <c r="J32" s="4">
         <v>4</v>
       </c>
@@ -3867,28 +3891,28 @@
       <c r="L32" s="4">
         <v>7.801258773512032E-2</v>
       </c>
-      <c r="M32" s="48">
-        <f t="shared" si="0"/>
+      <c r="M32" s="46">
+        <f t="shared" si="1"/>
         <v>62.89678927185436</v>
       </c>
-      <c r="N32" s="48">
+      <c r="N32" s="46">
         <v>68</v>
       </c>
-      <c r="O32" s="48">
-        <f t="shared" si="1"/>
+      <c r="O32" s="46">
+        <f t="shared" si="2"/>
         <v>-5.1032107281456405</v>
       </c>
-      <c r="P32" s="48">
-        <f t="shared" si="2"/>
+      <c r="P32" s="46">
+        <f t="shared" si="3"/>
         <v>5.1032107281456405</v>
       </c>
-      <c r="Q32" s="49">
-        <f t="shared" si="3"/>
+      <c r="Q32" s="47">
+        <f t="shared" si="4"/>
         <v>7.5047216590377067E-2</v>
       </c>
     </row>
     <row r="33" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F33" s="33"/>
+      <c r="F33" s="32"/>
       <c r="J33" s="4">
         <v>5</v>
       </c>
@@ -3898,28 +3922,28 @@
       <c r="L33" s="4">
         <v>-0.16147216203088011</v>
       </c>
-      <c r="M33" s="48">
-        <f t="shared" si="0"/>
+      <c r="M33" s="46">
+        <f t="shared" si="1"/>
         <v>84.617261381906175</v>
       </c>
-      <c r="N33" s="48">
+      <c r="N33" s="46">
         <v>72</v>
       </c>
-      <c r="O33" s="48">
-        <f t="shared" si="1"/>
-        <v>12.617261381906175</v>
-      </c>
-      <c r="P33" s="48">
+      <c r="O33" s="46">
         <f t="shared" si="2"/>
         <v>12.617261381906175</v>
       </c>
-      <c r="Q33" s="49">
+      <c r="P33" s="46">
         <f t="shared" si="3"/>
+        <v>12.617261381906175</v>
+      </c>
+      <c r="Q33" s="47">
+        <f t="shared" si="4"/>
         <v>0.17523974141536355</v>
       </c>
     </row>
     <row r="34" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F34" s="33"/>
+      <c r="F34" s="32"/>
       <c r="J34" s="4">
         <v>6</v>
       </c>
@@ -3929,28 +3953,28 @@
       <c r="L34" s="4">
         <v>6.6031741867249139E-2</v>
       </c>
-      <c r="M34" s="48">
-        <f t="shared" si="0"/>
+      <c r="M34" s="46">
+        <f t="shared" si="1"/>
         <v>76.760294318170338</v>
       </c>
-      <c r="N34" s="48">
+      <c r="N34" s="46">
         <v>82</v>
       </c>
-      <c r="O34" s="48">
-        <f t="shared" si="1"/>
+      <c r="O34" s="46">
+        <f t="shared" si="2"/>
         <v>-5.2397056818296619</v>
       </c>
-      <c r="P34" s="48">
-        <f t="shared" si="2"/>
+      <c r="P34" s="46">
+        <f t="shared" si="3"/>
         <v>5.2397056818296619</v>
       </c>
-      <c r="Q34" s="49">
-        <f t="shared" si="3"/>
+      <c r="Q34" s="47">
+        <f t="shared" si="4"/>
         <v>6.389884977841051E-2</v>
       </c>
     </row>
     <row r="35" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F35" s="33"/>
+      <c r="F35" s="32"/>
       <c r="J35" s="4">
         <v>7</v>
       </c>
@@ -3960,28 +3984,28 @@
       <c r="L35" s="4">
         <v>0.10455761540721475</v>
       </c>
-      <c r="M35" s="48">
-        <f t="shared" si="0"/>
+      <c r="M35" s="46">
+        <f t="shared" si="1"/>
         <v>77.462169433984585</v>
       </c>
-      <c r="N35" s="48">
+      <c r="N35" s="46">
         <v>86</v>
       </c>
-      <c r="O35" s="48">
-        <f t="shared" si="1"/>
+      <c r="O35" s="46">
+        <f t="shared" si="2"/>
         <v>-8.5378305660154155</v>
       </c>
-      <c r="P35" s="48">
-        <f t="shared" si="2"/>
+      <c r="P35" s="46">
+        <f t="shared" si="3"/>
         <v>8.5378305660154155</v>
       </c>
-      <c r="Q35" s="49">
-        <f t="shared" si="3"/>
+      <c r="Q35" s="47">
+        <f t="shared" si="4"/>
         <v>9.9277099604830416E-2</v>
       </c>
     </row>
     <row r="36" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F36" s="33"/>
+      <c r="F36" s="32"/>
       <c r="J36" s="4">
         <v>8</v>
       </c>
@@ -3991,28 +4015,28 @@
       <c r="L36" s="4">
         <v>1.3628077376804271E-2</v>
       </c>
-      <c r="M36" s="48">
-        <f t="shared" si="0"/>
+      <c r="M36" s="46">
+        <f t="shared" si="1"/>
         <v>85.822399707879697</v>
       </c>
-      <c r="N36" s="48">
+      <c r="N36" s="46">
         <v>87</v>
       </c>
-      <c r="O36" s="48">
-        <f t="shared" si="1"/>
+      <c r="O36" s="46">
+        <f t="shared" si="2"/>
         <v>-1.177600292120303</v>
       </c>
-      <c r="P36" s="48">
-        <f t="shared" si="2"/>
+      <c r="P36" s="46">
+        <f t="shared" si="3"/>
         <v>1.177600292120303</v>
       </c>
-      <c r="Q36" s="49">
-        <f t="shared" si="3"/>
+      <c r="Q36" s="47">
+        <f t="shared" si="4"/>
         <v>1.3535635541612679E-2</v>
       </c>
     </row>
     <row r="37" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F37" s="33"/>
+      <c r="F37" s="32"/>
       <c r="J37" s="4">
         <v>9</v>
       </c>
@@ -4022,28 +4046,28 @@
       <c r="L37" s="4">
         <v>8.7386872240061919E-2</v>
       </c>
-      <c r="M37" s="48">
-        <f t="shared" si="0"/>
+      <c r="M37" s="46">
+        <f t="shared" si="1"/>
         <v>83.385349984527096</v>
       </c>
-      <c r="N37" s="48">
+      <c r="N37" s="46">
         <v>91</v>
       </c>
-      <c r="O37" s="48">
-        <f t="shared" si="1"/>
+      <c r="O37" s="46">
+        <f t="shared" si="2"/>
         <v>-7.614650015472904</v>
       </c>
-      <c r="P37" s="48">
-        <f t="shared" si="2"/>
+      <c r="P37" s="46">
+        <f t="shared" si="3"/>
         <v>7.614650015472904</v>
       </c>
-      <c r="Q37" s="49">
-        <f t="shared" si="3"/>
+      <c r="Q37" s="47">
+        <f t="shared" si="4"/>
         <v>8.3677472697504446E-2</v>
       </c>
     </row>
     <row r="38" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F38" s="33"/>
+      <c r="F38" s="32"/>
       <c r="J38" s="4">
         <v>10</v>
       </c>
@@ -4053,28 +4077,28 @@
       <c r="L38" s="4">
         <v>5.4023847976880646E-2</v>
       </c>
-      <c r="M38" s="48">
-        <f t="shared" si="0"/>
+      <c r="M38" s="46">
+        <f t="shared" si="1"/>
         <v>90.951313193494926</v>
       </c>
-      <c r="N38" s="48">
+      <c r="N38" s="46">
         <v>96</v>
       </c>
-      <c r="O38" s="48">
-        <f t="shared" si="1"/>
+      <c r="O38" s="46">
+        <f t="shared" si="2"/>
         <v>-5.0486868065050743</v>
       </c>
-      <c r="P38" s="48">
-        <f t="shared" si="2"/>
+      <c r="P38" s="46">
+        <f t="shared" si="3"/>
         <v>5.0486868065050743</v>
       </c>
-      <c r="Q38" s="49">
-        <f t="shared" si="3"/>
+      <c r="Q38" s="47">
+        <f t="shared" si="4"/>
         <v>5.259048756776119E-2</v>
       </c>
     </row>
     <row r="39" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F39" s="32"/>
+      <c r="F39" s="31"/>
       <c r="J39" s="4">
         <v>11</v>
       </c>
@@ -4084,23 +4108,23 @@
       <c r="L39" s="4">
         <v>-1.8002597215063254E-2</v>
       </c>
-      <c r="M39" s="48">
-        <f t="shared" si="0"/>
+      <c r="M39" s="46">
+        <f t="shared" si="1"/>
         <v>102.83472769892616</v>
       </c>
-      <c r="N39" s="48">
+      <c r="N39" s="46">
         <v>101</v>
       </c>
-      <c r="O39" s="48">
-        <f t="shared" si="1"/>
-        <v>1.8347276989261587</v>
-      </c>
-      <c r="P39" s="48">
+      <c r="O39" s="46">
         <f t="shared" si="2"/>
         <v>1.8347276989261587</v>
       </c>
-      <c r="Q39" s="49">
+      <c r="P39" s="46">
         <f t="shared" si="3"/>
+        <v>1.8347276989261587</v>
+      </c>
+      <c r="Q39" s="47">
+        <f t="shared" si="4"/>
         <v>1.8165620781447116E-2</v>
       </c>
     </row>
@@ -4114,138 +4138,138 @@
       <c r="L40" s="5">
         <v>-5.6944712058371039E-4</v>
       </c>
-      <c r="M40" s="50">
-        <f t="shared" si="0"/>
+      <c r="M40" s="48">
+        <f t="shared" si="1"/>
         <v>105.05980897506939</v>
       </c>
-      <c r="N40" s="50">
+      <c r="N40" s="48">
         <v>105</v>
       </c>
-      <c r="O40" s="50">
-        <f t="shared" si="1"/>
-        <v>5.9808975069387316E-2</v>
-      </c>
-      <c r="P40" s="50">
+      <c r="O40" s="48">
         <f t="shared" si="2"/>
         <v>5.9808975069387316E-2</v>
       </c>
-      <c r="Q40" s="51">
+      <c r="P40" s="48">
         <f t="shared" si="3"/>
+        <v>5.9808975069387316E-2</v>
+      </c>
+      <c r="Q40" s="49">
+        <f t="shared" si="4"/>
         <v>5.6960928637511731E-4</v>
       </c>
     </row>
     <row r="41" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P41" s="40" t="s">
+      <c r="P41" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="Q41" s="41">
+      <c r="Q41" s="39">
         <f>SUM(Q29:Q40)</f>
         <v>0.81780320490693326</v>
       </c>
     </row>
     <row r="42" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P43" s="40" t="s">
+      <c r="P43" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="Q43" s="42">
+      <c r="Q43" s="40">
         <f>Q41/12</f>
         <v>6.8150267075577767E-2</v>
       </c>
     </row>
     <row r="44" spans="6:17" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J44" s="40" t="s">
+      <c r="J44" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="K44" s="46">
+      <c r="K44" s="44">
         <v>80</v>
       </c>
     </row>
     <row r="45" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J46" s="57" t="s">
+      <c r="J46" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="K46" s="43">
+      <c r="K46" s="41">
         <f>EXP(K21)*K44^K22</f>
         <v>98.149282181507928</v>
       </c>
     </row>
     <row r="47" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="H48" s="52" t="s">
+      <c r="H48" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="I48" s="53"/>
-      <c r="J48" s="45">
+      <c r="I48" s="64"/>
+      <c r="J48" s="43">
         <f>VARA(B6:B17)*12</f>
         <v>6033</v>
       </c>
-      <c r="K48" s="36"/>
+      <c r="K48" s="34"/>
     </row>
     <row r="49" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H49" s="54" t="s">
+      <c r="H49" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="I49" s="55"/>
-      <c r="J49" s="44">
+      <c r="I49" s="62"/>
+      <c r="J49" s="42">
         <f>(1+1/12+((K44-AVERAGE(B6:B17))^2)/J48)^0.5</f>
         <v>1.1004431170534803</v>
       </c>
-      <c r="K49" s="38"/>
+      <c r="K49" s="36"/>
     </row>
     <row r="50" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H50" s="54" t="s">
+      <c r="H50" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="I50" s="55"/>
-      <c r="J50" s="44">
+      <c r="I50" s="62"/>
+      <c r="J50" s="42">
         <f>K11*J49</f>
         <v>9.9654522649181121E-2</v>
       </c>
-      <c r="K50" s="38"/>
+      <c r="K50" s="36"/>
     </row>
     <row r="51" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H51" s="54" t="s">
+      <c r="H51" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="I51" s="55"/>
-      <c r="J51" s="44">
+      <c r="I51" s="62"/>
+      <c r="J51" s="42">
         <f>_xlfn.T.INV.2T(0.05,10)</f>
         <v>2.2281388519862744</v>
       </c>
-      <c r="K51" s="38"/>
+      <c r="K51" s="36"/>
     </row>
     <row r="52" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H52" s="54" t="s">
+      <c r="H52" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="I52" s="55"/>
-      <c r="J52" s="44">
+      <c r="I52" s="62"/>
+      <c r="J52" s="42">
         <f>J51*J50</f>
         <v>0.22204411369078661</v>
       </c>
-      <c r="K52" s="38"/>
+      <c r="K52" s="36"/>
     </row>
     <row r="53" spans="8:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H53" s="56" t="s">
+      <c r="H53" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="I53" s="58">
+      <c r="I53" s="52">
         <f>K46-J52</f>
         <v>97.927238067817143</v>
       </c>
-      <c r="J53" s="59" t="s">
+      <c r="J53" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="K53" s="60">
+      <c r="K53" s="54">
         <f>K46+J52</f>
         <v>98.371326295198713</v>
       </c>
     </row>
     <row r="58" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4258,4 +4282,31 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63500799-8A38-46C7-B88A-68046DC62E5B}">
+  <dimension ref="D7:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>22.9/4.4</f>
+        <v>5.2045454545454541</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>22.9/1.6</f>
+        <v>14.312499999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add `task-2` in `econometrics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-1/task-1.xlsx
+++ b/3-course-6-semester/econometrics/task-1/task-1.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\econometrics\task-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659854B9-9368-4AAB-8785-0630DF92E40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14E5E6F-01FB-4542-9C3B-44BBF244B397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{110B23AD-468D-4208-8880-E2E080976DA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{110B23AD-468D-4208-8880-E2E080976DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Занятие 1" sheetId="1" r:id="rId1"/>
     <sheet name="Домашнее задание 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3253,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63023E1B-49CB-46E7-86D3-D8D6E5AAD37A}">
   <dimension ref="B3:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4282,31 +4281,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63500799-8A38-46C7-B88A-68046DC62E5B}">
-  <dimension ref="D7:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <f>22.9/4.4</f>
-        <v>5.2045454545454541</v>
-      </c>
-    </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <f>22.9/1.6</f>
-        <v>14.312499999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>